<commit_message>
Final fix: clean requirements and add render.yaml
</commit_message>
<xml_diff>
--- a/processed/sentiment analysis test_with_sentiment.xlsx
+++ b/processed/sentiment analysis test_with_sentiment.xlsx
@@ -549,7 +549,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -955,7 +955,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>POSITIVE</t>
         </is>
       </c>
     </row>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>POSITIVE</t>
         </is>
       </c>
     </row>

</xml_diff>